<commit_message>
Data Collection Phase 1 Completed
</commit_message>
<xml_diff>
--- a/Raspi-Code/dweeter-run1.xlsx
+++ b/Raspi-Code/dweeter-run1.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="37470" windowHeight="18690"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37470" windowHeight="18690"/>
   </bookViews>
   <sheets>
     <sheet name="dweeter-run1.xls" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -914,11 +914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1134220704"/>
-        <c:axId val="949206672"/>
+        <c:axId val="-2113355744"/>
+        <c:axId val="-1925270400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1134220704"/>
+        <c:axId val="-2113355744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +960,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949206672"/>
+        <c:crossAx val="-1925270400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -968,7 +968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="949206672"/>
+        <c:axId val="-1925270400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,7 +1019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1134220704"/>
+        <c:crossAx val="-2113355744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1375,11 +1375,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="949318592"/>
-        <c:axId val="1327087568"/>
+        <c:axId val="-1924885424"/>
+        <c:axId val="-1924887600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="949318592"/>
+        <c:axId val="-1924885424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,7 +1421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327087568"/>
+        <c:crossAx val="-1924887600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1429,7 +1429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1327087568"/>
+        <c:axId val="-1924887600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1480,7 +1480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="949318592"/>
+        <c:crossAx val="-1924885424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1836,11 +1836,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1238976352"/>
-        <c:axId val="1238976896"/>
+        <c:axId val="-1925261696"/>
+        <c:axId val="-1925262784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1238976352"/>
+        <c:axId val="-1925261696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,7 +1882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238976896"/>
+        <c:crossAx val="-1925262784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1890,7 +1890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1238976896"/>
+        <c:axId val="-1925262784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,7 +1941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238976352"/>
+        <c:crossAx val="-1925261696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2297,11 +2297,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1238970368"/>
-        <c:axId val="1238970912"/>
+        <c:axId val="-1925260608"/>
+        <c:axId val="-1925261152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1238970368"/>
+        <c:axId val="-1925260608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2343,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238970912"/>
+        <c:crossAx val="-1925261152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2351,7 +2351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1238970912"/>
+        <c:axId val="-1925261152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238970368"/>
+        <c:crossAx val="-1925260608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2758,11 +2758,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1238967104"/>
-        <c:axId val="1238967648"/>
+        <c:axId val="-1925271488"/>
+        <c:axId val="-1925274752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1238967104"/>
+        <c:axId val="-1925271488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2804,7 +2804,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238967648"/>
+        <c:crossAx val="-1925274752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2812,7 +2812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1238967648"/>
+        <c:axId val="-1925274752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2863,7 +2863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238967104"/>
+        <c:crossAx val="-1925271488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3219,11 +3219,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1238969280"/>
-        <c:axId val="1238969824"/>
+        <c:axId val="-1925272576"/>
+        <c:axId val="-1925263872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1238969280"/>
+        <c:axId val="-1925272576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,7 +3265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238969824"/>
+        <c:crossAx val="-1925263872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3273,7 +3273,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1238969824"/>
+        <c:axId val="-1925263872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3324,7 +3324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238969280"/>
+        <c:crossAx val="-1925272576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3680,11 +3680,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1327088112"/>
-        <c:axId val="1327092464"/>
+        <c:axId val="-1925263328"/>
+        <c:axId val="-1925264416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1327088112"/>
+        <c:axId val="-1925263328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,7 +3726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327092464"/>
+        <c:crossAx val="-1925264416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3734,7 +3734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1327092464"/>
+        <c:axId val="-1925264416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3785,7 +3785,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327088112"/>
+        <c:crossAx val="-1925263328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4141,11 +4141,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1327081584"/>
-        <c:axId val="1327094640"/>
+        <c:axId val="-1925268224"/>
+        <c:axId val="-1925267680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1327081584"/>
+        <c:axId val="-1925268224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4187,7 +4187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327094640"/>
+        <c:crossAx val="-1925267680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4195,7 +4195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1327094640"/>
+        <c:axId val="-1925267680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4246,7 +4246,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327081584"/>
+        <c:crossAx val="-1925268224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4602,11 +4602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1327093008"/>
-        <c:axId val="1327095184"/>
+        <c:axId val="-1925266048"/>
+        <c:axId val="-1925264960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1327093008"/>
+        <c:axId val="-1925266048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4648,7 +4648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327095184"/>
+        <c:crossAx val="-1925264960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4656,7 +4656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1327095184"/>
+        <c:axId val="-1925264960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4707,7 +4707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327093008"/>
+        <c:crossAx val="-1925266048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5063,11 +5063,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1327083216"/>
-        <c:axId val="1327083760"/>
+        <c:axId val="-1924885968"/>
+        <c:axId val="-1924882704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1327083216"/>
+        <c:axId val="-1924885968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5109,7 +5109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327083760"/>
+        <c:crossAx val="-1924882704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5117,7 +5117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1327083760"/>
+        <c:axId val="-1924882704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5168,7 +5168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1327083216"/>
+        <c:crossAx val="-1924885968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>